<commit_message>
Search Listing page added one more steps
</commit_message>
<xml_diff>
--- a/src/main/java/com/bigbasket/testdata/Test Suite1.xlsx
+++ b/src/main/java/com/bigbasket/testdata/Test Suite1.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Test Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="B1:H10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>TCID</t>
   </si>
@@ -74,6 +73,15 @@
   </si>
   <si>
     <t>apple</t>
+  </si>
+  <si>
+    <t>addProduct</t>
+  </si>
+  <si>
+    <t>search_list_projectNames|search_list_addBtn</t>
+  </si>
+  <si>
+    <t>Apple - Royal Gala</t>
   </si>
 </sst>
 </file>
@@ -491,10 +499,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -627,6 +635,21 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more project added in basket test cases
</commit_message>
<xml_diff>
--- a/src/main/java/com/bigbasket/testdata/Test Suite1.xlsx
+++ b/src/main/java/com/bigbasket/testdata/Test Suite1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
   <si>
     <t>TCID</t>
   </si>
@@ -82,6 +82,24 @@
   </si>
   <si>
     <t>Apple - Royal Gala</t>
+  </si>
+  <si>
+    <t>verifyText</t>
+  </si>
+  <si>
+    <t>productName_text</t>
+  </si>
+  <si>
+    <t>product_add_btn</t>
+  </si>
+  <si>
+    <t>search_list_footerpage</t>
+  </si>
+  <si>
+    <t>goBack</t>
+  </si>
+  <si>
+    <t>Green Apple</t>
   </si>
 </sst>
 </file>
@@ -499,10 +517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -602,7 +620,7 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
@@ -615,14 +633,12 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
@@ -630,9 +646,11 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
@@ -643,14 +661,122 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>